<commit_message>
finished linear 1y prototype model
</commit_message>
<xml_diff>
--- a/analysis/data/corr_pearson_-1y.xlsx
+++ b/analysis/data/corr_pearson_-1y.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\stei509\eu_migration_forecast\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E765FA13-21CD-4C00-885A-3903FE1855A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208CCCDE-0F1F-4E16-9FEF-71E85AB2BC92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,6 +263,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +310,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -617,13 +646,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL18" sqref="AL18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +798,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -909,7 +938,7 @@
         <v>0.5162647636921549</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -1055,7 +1084,7 @@
         <v>-0.93874190151416781</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1201,7 +1230,7 @@
         <v>-5.6485833763759541E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1347,7 +1376,7 @@
         <v>-9.7116578546504129E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -1484,7 +1513,7 @@
         <v>-0.30301110211859911</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -1582,7 +1611,7 @@
         <v>0.84474140858405478</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -1725,7 +1754,7 @@
         <v>0.64717190635086719</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -1832,7 +1861,7 @@
         <v>0.31343884983958969</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -1924,7 +1953,7 @@
         <v>0.52878744611026285</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
@@ -2001,7 +2030,7 @@
         <v>0.32968609119235393</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2090,7 +2119,7 @@
         <v>-7.8282229143097626E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -2191,7 +2220,7 @@
         <v>0.84800918220528587</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -2280,7 +2309,7 @@
         <v>-0.17195920531805189</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
@@ -2420,7 +2449,7 @@
         <v>0.17826868045722211</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -2566,7 +2595,7 @@
         <v>0.89393443562418973</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2655,7 +2684,7 @@
         <v>0.86351613320025888</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -2747,7 +2776,7 @@
         <v>0.56327540740836324</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -2812,7 +2841,7 @@
         <v>-0.10916827149003271</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -2865,7 +2894,7 @@
         <v>-0.1348078759419947</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -2957,7 +2986,7 @@
         <v>0.23823040449094579</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -3019,7 +3048,7 @@
         <v>0.87914630438791574</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -3069,7 +3098,7 @@
         <v>0.48351056261431669</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -3116,7 +3145,7 @@
         <v>-0.11076630938755171</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3163,7 +3192,7 @@
         <v>-0.52891418085110753</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3207,7 +3236,7 @@
         <v>-0.46236155021011838</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3260,7 +3289,7 @@
         <v>-0.63950301065065729</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
@@ -3324,8 +3353,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AW28">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0.62</formula>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0.63</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>-0.63</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>